<commit_message>
Added multipage Fixed spelling error Added code to create report
</commit_message>
<xml_diff>
--- a/Archery.Template.xlsx
+++ b/Archery.Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Dropbox\Archersoft\Dapug\Dapug 20250318\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CAA5DD-770B-4F29-938F-FABD267417AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC0ED8F-54D6-462C-8148-B0621B5E4D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25965" yWindow="2085" windowWidth="25665" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26790" yWindow="3105" windowWidth="25665" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -46,10 +46,10 @@
     <t>Results</t>
   </si>
   <si>
-    <t>&lt;#ARCHERRESULT.COMPETITIONNAME&gt;</t>
-  </si>
-  <si>
-    <t>&lt;#ARCHERRESULT.COMPETITIONRESULT&gt;</t>
+    <t>&lt;#RESULTS.COMPETITIONRESULT&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#RESULTS.COMPETITIONNAME&gt;</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
   <dimension ref="B4:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,10 +394,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
         <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>